<commit_message>
Added SVR parameter loading from pred_par structure and Excel files
</commit_message>
<xml_diff>
--- a/Time_series_forecasting/a. Input time series sequences/Ext markers seq 1  3.33 Hz/pred_par.xlsx
+++ b/Time_series_forecasting/a. Input time series sequences/Ext markers seq 1  3.33 Hz/pred_par.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96280BC9-0C91-4E69-BCC2-561E309015E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0E0CD8-BB51-400E-934D-D5227FD63DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Remarks :</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>data_type : 1 -&gt; position of 3D markers / 2 -&gt; PCA components of DVF</t>
+  </si>
+  <si>
+    <t>svr_kernel_scale</t>
+  </si>
+  <si>
+    <t>svr_epsilon</t>
+  </si>
+  <si>
+    <t>svr_box_constraint</t>
   </si>
 </sst>
 </file>
@@ -138,18 +147,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -165,9 +172,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -205,9 +212,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,26 +247,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,26 +282,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,35 +458,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K1" sqref="K1:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" customWidth="1"/>
     <col min="4" max="4" width="5.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="6" max="6" width="20.46484375" customWidth="1"/>
+    <col min="7" max="7" width="16.46484375" customWidth="1"/>
+    <col min="8" max="8" width="13.46484375" customWidth="1"/>
+    <col min="9" max="9" width="14.46484375" customWidth="1"/>
+    <col min="10" max="10" width="10.53125" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
@@ -522,13 +495,13 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
       <c r="I1" t="s">
@@ -537,30 +510,39 @@
       <c r="J1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
         <v>100</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>740</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>200</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>50</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>50</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>0.02</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
@@ -569,130 +551,138 @@
       <c r="J2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>0.2</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D19" s="1">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D19">
         <v>10</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>40</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>0.01</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19">
         <v>0.1</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D20" s="1">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D20">
         <v>25</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
         <v>55</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
         <v>0.01</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20">
         <v>0.1</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D21" s="1">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D21">
         <v>40</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21">
         <v>55</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21">
         <v>0.02</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21">
         <v>0.1</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D23">
         <v>40</v>
       </c>
@@ -706,8 +696,8 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D25" s="4"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>